<commit_message>
refatorando o código inteiro
Adicionados novas funções,

Estilizados as tabelas
Gerando o Dado mais limpo e fácil para tomada de decisão
</commit_message>
<xml_diff>
--- a/itens_mapeados_sem_expositor_cadastrado.xlsx
+++ b/itens_mapeados_sem_expositor_cadastrado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GABRIEL" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="THAINI" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="GABRIEL" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="THAINI" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>